<commit_message>
fix import templates (products and orders)
</commit_message>
<xml_diff>
--- a/public/OrderTemplate.xlsx
+++ b/public/OrderTemplate.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27307"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96202E3A-5988-064B-B747-FD5553530DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9524164-A044-400F-970C-4F80219F7C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="21100" tabRatio="471" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
   <si>
     <t>Order Number</t>
   </si>
@@ -67,9 +67,18 @@
     <t>Product Name</t>
   </si>
   <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Price currency</t>
+  </si>
+  <si>
     <t>COD</t>
   </si>
   <si>
+    <t>COD currency</t>
+  </si>
+  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -136,6 +145,12 @@
     <t>name of the item in the order</t>
   </si>
   <si>
+    <t>Price of one product item</t>
+  </si>
+  <si>
+    <t>Currency of the price (as in seller's store)</t>
+  </si>
+  <si>
     <t>cash on delivery amount (if it is a COD order)</t>
   </si>
   <si>
@@ -217,6 +232,9 @@
     <t>GBP</t>
   </si>
   <si>
+    <t>EUR</t>
+  </si>
+  <si>
     <t>sales</t>
   </si>
   <si>
@@ -251,19 +269,13 @@
   </si>
   <si>
     <t>Desert scarf</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>COD currency</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,40 +709,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.85546875" style="9" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.1640625" style="1"/>
+    <col min="20" max="20" width="18.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="25" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10" style="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -764,44 +779,50 @@
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="R1" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="U1" s="8" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="W1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="8" t="s">
         <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -812,37 +833,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E771F0C-1168-4963-95C7-BC373555E38F}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.5" style="12"/>
-    <col min="4" max="4" width="18.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="12" customWidth="1"/>
-    <col min="8" max="10" width="11.5" style="12"/>
-    <col min="11" max="11" width="16.5" style="12" customWidth="1"/>
-    <col min="12" max="13" width="11.5" style="13"/>
-    <col min="14" max="14" width="11.5" style="12"/>
-    <col min="15" max="15" width="18.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5" style="15" customWidth="1"/>
-    <col min="19" max="19" width="19.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13" style="13" customWidth="1"/>
-    <col min="24" max="24" width="11.5" style="15"/>
+    <col min="2" max="3" width="11.42578125" style="12"/>
+    <col min="4" max="4" width="18.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="12" customWidth="1"/>
+    <col min="8" max="10" width="11.42578125" style="12"/>
+    <col min="11" max="13" width="16.42578125" style="12" customWidth="1"/>
+    <col min="14" max="15" width="11.42578125" style="13"/>
+    <col min="16" max="16" width="11.42578125" style="12"/>
+    <col min="17" max="17" width="18.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" style="15" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13" style="13" customWidth="1"/>
+    <col min="26" max="26" width="11.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -876,340 +897,376 @@
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="O1" s="4"/>
+      <c r="P1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="2" customFormat="1" ht="159.94999999999999">
+      <c r="A2" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>22</v>
+      <c r="P2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="V2" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="21" t="s">
+        <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="2" customFormat="1" ht="160" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="18" t="s">
+    <row r="3" spans="1:26" s="2" customFormat="1" ht="63.95">
+      <c r="A3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="W3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="X3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y3" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z3" s="21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="32.1">
+      <c r="A4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="12">
         <v>33</v>
       </c>
-      <c r="L2" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="19" t="s">
+      <c r="M4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="15">
+        <v>100</v>
+      </c>
+      <c r="S4" s="15">
+        <v>0</v>
+      </c>
+      <c r="T4" s="15">
+        <v>0</v>
+      </c>
+      <c r="U4" s="15">
+        <v>10</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y4" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" s="15">
+        <v>457386927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="V2" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="U3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="W3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="N4" s="12">
-        <v>1</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" s="15">
-        <v>100</v>
-      </c>
-      <c r="Q4" s="15">
-        <v>0</v>
-      </c>
-      <c r="R4" s="15">
-        <v>0</v>
-      </c>
-      <c r="S4" s="15">
-        <v>10</v>
-      </c>
-      <c r="T4" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="W4" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="X4" s="15">
-        <v>457386927</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>68</v>
       </c>
       <c r="I5" s="17">
         <v>20122</v>
       </c>
       <c r="J5" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="L5" s="12">
+        <v>11</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N5" s="13">
+        <v>145</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="P5" s="12">
+        <v>2</v>
+      </c>
+      <c r="X5" s="13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="C6" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="13">
-        <v>145</v>
-      </c>
-      <c r="M5" s="13" t="s">
+      <c r="E6" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="N5" s="12">
-        <v>2</v>
-      </c>
-      <c r="V5" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>67</v>
-      </c>
       <c r="H6" s="12" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="I6" s="17">
         <v>20122</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="L6" s="13">
+        <v>78</v>
+      </c>
+      <c r="L6" s="12">
+        <v>18</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N6" s="13">
         <v>300</v>
       </c>
-      <c r="M6" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="N6" s="12">
+      <c r="O6" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="12">
         <v>1</v>
       </c>
-      <c r="V6" s="13" t="s">
-        <v>71</v>
+      <c r="X6" s="13" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1220,4 +1277,219 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100505376291F6FC345B254CE62B25F476D" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2261d02df530edde1c157d25699d65ff">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="595e45d7-2eb9-4664-b98e-ad279a82e308" xmlns:ns3="e65950c5-8261-4459-8a02-867ddf65e5f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84b3faa87fc3e2bc73449ee0be32afcc" ns2:_="" ns3:_="">
+    <xsd:import namespace="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
+    <xsd:import namespace="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="595e45d7-2eb9-4664-b98e-ad279a82e308" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="9" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b9506e52-7e6f-4938-8c0d-0e8b16a3f561" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="13" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e65950c5-8261-4459-8a02-867ddf65e5f1" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="10" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{f2a168f5-0a39-4c60-9222-68737c9f6dd5}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="e65950c5-8261-4459-8a02-867ddf65e5f1">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="595e45d7-2eb9-4664-b98e-ad279a82e308">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e65950c5-8261-4459-8a02-867ddf65e5f1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53764236-501A-424B-B104-68FAA79E0A9F}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64A857A-C759-4F0E-970D-B1D1C317D486}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D913A73D-BD4E-4573-BA03-F7E0ADC6E020}"/>
 </file>
</xml_diff>

<commit_message>
fix reports and product selection, add new order template
</commit_message>
<xml_diff>
--- a/public/OrderTemplate.xlsx
+++ b/public/OrderTemplate.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27307"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9524164-A044-400F-970C-4F80219F7C57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB96A9C-44EC-714D-86F3-C1639FFE9B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="21100" tabRatio="471" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="TO BE FILLED" sheetId="1" r:id="rId1"/>
     <sheet name="FILLING RULES AND EXAMPLE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
   <si>
     <t>Order Number</t>
   </si>
@@ -269,13 +269,19 @@
   </si>
   <si>
     <t>Desert scarf</t>
+  </si>
+  <si>
+    <t>PreferredDeliveryDate</t>
+  </si>
+  <si>
+    <t>date when the order should be delivered</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,7 +374,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -428,6 +434,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -709,43 +716,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.85546875" style="9" customWidth="1"/>
-    <col min="14" max="14" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.83203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5" style="11" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" style="11" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.140625" style="1"/>
+    <col min="27" max="27" width="24.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -823,6 +831,9 @@
       </c>
       <c r="Z1" s="8" t="s">
         <v>25</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -833,37 +844,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E771F0C-1168-4963-95C7-BC373555E38F}">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.42578125" style="12"/>
-    <col min="4" max="4" width="18.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="12" customWidth="1"/>
-    <col min="8" max="10" width="11.42578125" style="12"/>
-    <col min="11" max="13" width="16.42578125" style="12" customWidth="1"/>
-    <col min="14" max="15" width="11.42578125" style="13"/>
-    <col min="16" max="16" width="11.42578125" style="12"/>
-    <col min="17" max="17" width="18.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.42578125" style="15" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.5" style="12"/>
+    <col min="4" max="4" width="18.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" style="12" customWidth="1"/>
+    <col min="8" max="10" width="11.5" style="12"/>
+    <col min="11" max="13" width="16.5" style="12" customWidth="1"/>
+    <col min="14" max="15" width="11.5" style="13"/>
+    <col min="16" max="16" width="11.5" style="12"/>
+    <col min="17" max="17" width="18.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5" style="15" customWidth="1"/>
+    <col min="21" max="21" width="19.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="13" style="13" customWidth="1"/>
-    <col min="26" max="26" width="11.42578125" style="15"/>
+    <col min="26" max="26" width="11.5" style="15"/>
+    <col min="27" max="27" width="19.5" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -940,8 +952,11 @@
       <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" s="2" customFormat="1" ht="159.94999999999999">
+    <row r="2" spans="1:27" s="2" customFormat="1" ht="160" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
@@ -1020,8 +1035,11 @@
       <c r="Z2" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="AA2" s="19" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" s="2" customFormat="1" ht="63.95">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>51</v>
       </c>
@@ -1100,8 +1118,11 @@
       <c r="Z3" s="21" t="s">
         <v>54</v>
       </c>
+      <c r="AA3" s="19" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" ht="32.1">
+    <row r="4" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>55</v>
       </c>
@@ -1169,7 +1190,7 @@
         <v>457386927</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>68</v>
       </c>
@@ -1218,8 +1239,11 @@
       <c r="X5" s="13" t="s">
         <v>77</v>
       </c>
+      <c r="AA5" s="22">
+        <v>45533</v>
+      </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>68</v>
       </c>
@@ -1289,6 +1313,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="595e45d7-2eb9-4664-b98e-ad279a82e308">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e65950c5-8261-4459-8a02-867ddf65e5f1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100505376291F6FC345B254CE62B25F476D" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2261d02df530edde1c157d25699d65ff">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="595e45d7-2eb9-4664-b98e-ad279a82e308" xmlns:ns3="e65950c5-8261-4459-8a02-867ddf65e5f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84b3faa87fc3e2bc73449ee0be32afcc" ns2:_="" ns3:_="">
     <xsd:import namespace="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
@@ -1471,25 +1506,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="595e45d7-2eb9-4664-b98e-ad279a82e308">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e65950c5-8261-4459-8a02-867ddf65e5f1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53764236-501A-424B-B104-68FAA79E0A9F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53764236-501A-424B-B104-68FAA79E0A9F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64A857A-C759-4F0E-970D-B1D1C317D486}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D913A73D-BD4E-4573-BA03-F7E0ADC6E020}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
+    <ds:schemaRef ds:uri="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D913A73D-BD4E-4573-BA03-F7E0ADC6E020}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64A857A-C759-4F0E-970D-B1D1C317D486}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
+    <ds:schemaRef ds:uri="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change Order template (added CourierService and Warehouse + Mandatory)
</commit_message>
<xml_diff>
--- a/public/OrderTemplate.xlsx
+++ b/public/OrderTemplate.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB96A9C-44EC-714D-86F3-C1639FFE9B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{009CED6B-08BC-4420-910C-7777398F2D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="21100" tabRatio="471" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" tabRatio="471" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TO BE FILLED" sheetId="1" r:id="rId1"/>
     <sheet name="FILLING RULES AND EXAMPLE" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -23,7 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
   <si>
     <t>Order Number</t>
   </si>
@@ -103,13 +103,16 @@
     <t>CourierService</t>
   </si>
   <si>
-    <t>CommentForCourier</t>
-  </si>
-  <si>
-    <t>ContactPerson</t>
-  </si>
-  <si>
-    <t>VatEori</t>
+    <t>Mandatory CourierService</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Mandatory Warehouse</t>
+  </si>
+  <si>
+    <t>PreferredDeliveryDate</t>
   </si>
   <si>
     <t>order number in the seller's system or just convenient</t>
@@ -175,16 +178,19 @@
     <t>basis for export in a free form</t>
   </si>
   <si>
-    <t>courier service name</t>
-  </si>
-  <si>
-    <t>comment for courier service (works not in all countries)</t>
-  </si>
-  <si>
-    <t>contacts of the person receiving the parcel</t>
-  </si>
-  <si>
-    <t>taxable person number / registration and identification number of the economic operator</t>
+    <t>name of preferred courier service, if the parcel can't be shipped by specified courier service, the system will decide which courier service will deliver the parcel</t>
+  </si>
+  <si>
+    <t>if you specify as true - this courier service will be considered as priority</t>
+  </si>
+  <si>
+    <t>code of the warehouse if you want to choose this warehouse for sending your parcel</t>
+  </si>
+  <si>
+    <t>if you specify as true - this warehouse will be considered as priority</t>
+  </si>
+  <si>
+    <t>date when the order should be delivered</t>
   </si>
   <si>
     <t>required</t>
@@ -238,6 +244,15 @@
     <t>sales</t>
   </si>
   <si>
+    <t>CorreosExpress</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>ITWH6</t>
+  </si>
+  <si>
     <t>1119-lvx</t>
   </si>
   <si>
@@ -265,23 +280,17 @@
     <t>Magic Glove</t>
   </si>
   <si>
-    <t>Please call before delivery</t>
-  </si>
-  <si>
     <t>Desert scarf</t>
   </si>
   <si>
-    <t>PreferredDeliveryDate</t>
-  </si>
-  <si>
-    <t>date when the order should be delivered</t>
+    <t>false</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -435,6 +444,16 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -718,42 +737,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.83203125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="6.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="17.85546875" style="9" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.6640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.83203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.1640625" style="1"/>
+    <col min="22" max="22" width="21.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26" style="10" customWidth="1"/>
+    <col min="24" max="24" width="24.28515625" style="10" customWidth="1"/>
+    <col min="25" max="25" width="22.85546875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="23.7109375" style="10" customWidth="1"/>
+    <col min="27" max="27" width="24.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -829,16 +848,28 @@
       <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5705583C-A9F2-E34B-9EE8-C1DC9DCDAE43}">
+          <x14:formula1>
+            <xm:f>Лист1!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z2:Z1048576 X2:X1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -846,36 +877,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E771F0C-1168-4963-95C7-BC373555E38F}">
   <dimension ref="A1:AA6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AA6" sqref="AA6"/>
+    <sheetView topLeftCell="U1" zoomScale="150" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y5" sqref="Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.5" style="12"/>
-    <col min="4" max="4" width="18.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="12" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" style="12" customWidth="1"/>
-    <col min="8" max="10" width="11.5" style="12"/>
-    <col min="11" max="13" width="16.5" style="12" customWidth="1"/>
-    <col min="14" max="15" width="11.5" style="13"/>
-    <col min="16" max="16" width="11.5" style="12"/>
-    <col min="17" max="17" width="18.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5" style="15" customWidth="1"/>
-    <col min="21" max="21" width="19.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" style="13" customWidth="1"/>
-    <col min="26" max="26" width="11.5" style="15"/>
-    <col min="27" max="27" width="19.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="12"/>
+    <col min="4" max="4" width="18.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="12" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="12" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="12" customWidth="1"/>
+    <col min="8" max="10" width="11.42578125" style="12"/>
+    <col min="11" max="13" width="16.42578125" style="12" customWidth="1"/>
+    <col min="14" max="15" width="11.42578125" style="13"/>
+    <col min="16" max="16" width="11.42578125" style="12"/>
+    <col min="17" max="17" width="18.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.42578125" style="15" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.85546875" style="10" customWidth="1"/>
+    <col min="24" max="24" width="24.28515625" style="10" customWidth="1"/>
+    <col min="25" max="25" width="22.85546875" style="10" customWidth="1"/>
+    <col min="26" max="26" width="23.7109375" style="10" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -949,224 +980,224 @@
       <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>79</v>
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="2" customFormat="1" ht="160" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" s="2" customFormat="1" ht="111.95">
       <c r="A2" s="18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N2" s="19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O2" s="19" t="s">
         <v>14</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Q2" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="W2" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="W2" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="19" t="s">
+      <c r="X2" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="21" t="s">
+      <c r="Y2" s="24" t="s">
         <v>50</v>
       </c>
+      <c r="Z2" s="24" t="s">
+        <v>51</v>
+      </c>
       <c r="AA2" s="19" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" s="2" customFormat="1" ht="48">
       <c r="A3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="K3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="N3" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="O3" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="18" t="s">
-        <v>51</v>
-      </c>
       <c r="Q3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="W3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="R3" s="21" t="s">
+      <c r="X3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="21" t="s">
+      <c r="Y3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="T3" s="21" t="s">
+      <c r="Z3" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="AA3" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="V3" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="W3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="X3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y3" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="Z3" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA3" s="19" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="4" spans="1:27" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="32.1">
       <c r="A4" s="12" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L4" s="12">
         <v>33</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O4" s="13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P4" s="12">
         <v>1</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="R4" s="15">
         <v>100</v>
@@ -1181,116 +1212,121 @@
         <v>10</v>
       </c>
       <c r="V4" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z4" s="15">
-        <v>457386927</v>
+        <v>69</v>
+      </c>
+      <c r="W4" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="X4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y4" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA4" s="22">
+        <v>45533</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27">
       <c r="A5" s="12" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I5" s="17">
         <v>20122</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="L5" s="12">
         <v>11</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N5" s="13">
         <v>145</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P5" s="12">
         <v>2</v>
       </c>
-      <c r="X5" s="13" t="s">
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="22"/>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="AA5" s="22">
-        <v>45533</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>72</v>
-      </c>
       <c r="G6" s="12" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I6" s="17">
         <v>20122</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L6" s="12">
         <v>18</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N6" s="13">
         <v>300</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P6" s="12">
         <v>1</v>
-      </c>
-      <c r="X6" s="13" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1300,10 +1336,64 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="true" xr:uid="{B2B4F942-8302-2945-A380-2CED55ACB968}">
+          <x14:formula1>
+            <xm:f>Лист1!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>X4:X9 X11:X1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3467A637-F298-3042-8DA1-083E2090B6D2}">
+          <x14:formula1>
+            <xm:f>Лист1!$A$1:$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z5:Z1048576 Z4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C554B4-578E-D24C-B026-7E370BD231B1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.95">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.95">
+      <c r="A2" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="61fb5273-9fa9-47b1-aee4-88cf85ecd011">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="b81398df-9a3a-473d-8e44-cc5041003447" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1312,36 +1402,28 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="595e45d7-2eb9-4664-b98e-ad279a82e308">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e65950c5-8261-4459-8a02-867ddf65e5f1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100505376291F6FC345B254CE62B25F476D" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2261d02df530edde1c157d25699d65ff">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="595e45d7-2eb9-4664-b98e-ad279a82e308" xmlns:ns3="e65950c5-8261-4459-8a02-867ddf65e5f1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="84b3faa87fc3e2bc73449ee0be32afcc" ns2:_="" ns3:_="">
-    <xsd:import namespace="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
-    <xsd:import namespace="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Документ" ma:contentTypeID="0x0101004E609D4606550E41B3933AD7C596A883" ma:contentTypeVersion="12" ma:contentTypeDescription="Создание документа." ma:contentTypeScope="" ma:versionID="360ee472c2c8273e109d420e398f1f4f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="61fb5273-9fa9-47b1-aee4-88cf85ecd011" xmlns:ns3="b81398df-9a3a-473d-8e44-cc5041003447" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="079f72354deb4dc42c47ed909bd058b3" ns2:_="" ns3:_="">
+    <xsd:import namespace="61fb5273-9fa9-47b1-aee4-88cf85ecd011"/>
+    <xsd:import namespace="b81398df-9a3a-473d-8e44-cc5041003447"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element name="documentManagement">
             <xsd:complexType>
               <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1349,53 +1431,68 @@
       </xsd:complexType>
     </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="595e45d7-2eb9-4664-b98e-ad279a82e308" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="61fb5273-9fa9-47b1-aee4-88cf85ecd011" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="9" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b9506e52-7e6f-4938-8c0d-0e8b16a3f561" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Теги изображений" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="b9506e52-7e6f-4938-8c0d-0e8b16a3f561" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="13" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+    <xsd:element name="MediaServiceDateTaken" ma:index="15" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="14" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+    <xsd:element name="MediaServiceOCR" ma:index="16" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="15" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="16" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
   </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e65950c5-8261-4459-8a02-867ddf65e5f1" elementFormDefault="qualified">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b81398df-9a3a-473d-8e44-cc5041003447" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="10" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{f2a168f5-0a39-4c60-9222-68737c9f6dd5}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="e65950c5-8261-4459-8a02-867ddf65e5f1">
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{efc9519b-137d-4e74-9f75-e409a3d4d103}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="b81398df-9a3a-473d-8e44-cc5041003447">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:MultiChoiceLookup">
@@ -1416,8 +1513,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Тип контента"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Название"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -1507,39 +1604,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53764236-501A-424B-B104-68FAA79E0A9F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D913A73D-BD4E-4573-BA03-F7E0ADC6E020}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D913A73D-BD4E-4573-BA03-F7E0ADC6E020}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
-    <ds:schemaRef ds:uri="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53764236-501A-424B-B104-68FAA79E0A9F}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E64A857A-C759-4F0E-970D-B1D1C317D486}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="595e45d7-2eb9-4664-b98e-ad279a82e308"/>
-    <ds:schemaRef ds:uri="e65950c5-8261-4459-8a02-867ddf65e5f1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27546932-B6DF-4587-89B1-21BF48488D22}"/>
 </file>
</xml_diff>